<commit_message>
status tracker update (18 feb)
</commit_message>
<xml_diff>
--- a/docs/status tracker.xlsx
+++ b/docs/status tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00CC1B8-473B-4D80-993F-E1388133C0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1119DA8-4ADC-4123-988B-02F4CBD2E3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="75">
   <si>
     <r>
       <rPr>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>Learn React</t>
-  </si>
-  <si>
-    <t>Week 6</t>
   </si>
   <si>
     <r>
@@ -225,12 +222,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Week 4(February 5-February 12)</t>
-  </si>
-  <si>
-    <t>Week 5 (February 13-February 20)</t>
-  </si>
-  <si>
     <t>Other Pages</t>
   </si>
   <si>
@@ -247,6 +238,51 @@
   </si>
   <si>
     <t>Discussion of what all pages we need to create</t>
+  </si>
+  <si>
+    <t>Week 4(February 5-February 11)</t>
+  </si>
+  <si>
+    <t>Week 5 (February 12-February 18)</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>Form Page</t>
+  </si>
+  <si>
+    <t>View Tools Page</t>
+  </si>
+  <si>
+    <t>Status Update Page</t>
+  </si>
+  <si>
+    <t>Aditya,Atidipt</t>
+  </si>
+  <si>
+    <t>Give updates about the work, and next thing we need to do</t>
+  </si>
+  <si>
+    <t>Discussion of what all work is done and what all needs to be done</t>
+  </si>
+  <si>
+    <t>Create a home page for the dashboard</t>
+  </si>
+  <si>
+    <t>Create a page where details of tools will be there</t>
+  </si>
+  <si>
+    <t>Create a page where all the tools ordered can be displayed</t>
+  </si>
+  <si>
+    <t>Track tools which are ordered</t>
+  </si>
+  <si>
+    <t>Week 6 (February 19-February 25)</t>
+  </si>
+  <si>
+    <t>Week 7 (February 26-March 3 )</t>
   </si>
 </sst>
 </file>
@@ -298,7 +334,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,12 +369,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -470,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -567,8 +597,8 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -579,15 +609,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -595,9 +616,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -927,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="98" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999"/>
@@ -1002,7 +1020,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>17</v>
@@ -1015,15 +1033,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A6" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
+      <c r="A6" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:7" ht="9" customHeight="1">
       <c r="A7" s="33" t="s">
@@ -1320,13 +1338,13 @@
         <v>0.5</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" s="29" t="s">
         <v>2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="9" customHeight="1">
@@ -1366,7 +1384,7 @@
         <v>6</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>3</v>
@@ -1389,7 +1407,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>3</v>
@@ -1412,7 +1430,7 @@
         <v>8</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F26" s="30" t="s">
         <v>3</v>
@@ -1423,7 +1441,7 @@
     </row>
     <row r="27" spans="1:7" ht="9" customHeight="1">
       <c r="A27" s="33" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
@@ -1452,12 +1470,12 @@
         <v>4</v>
       </c>
       <c r="G28" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="8.5500000000000007" customHeight="1">
       <c r="A29" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>1</v>
@@ -1475,7 +1493,7 @@
         <v>4</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="9" customHeight="1">
@@ -1512,7 +1530,7 @@
     </row>
     <row r="32" spans="1:7" ht="9" customHeight="1">
       <c r="A32" s="33" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B32" s="34"/>
       <c r="C32" s="34"/>
@@ -1534,14 +1552,14 @@
       <c r="D33" s="14">
         <v>0.5</v>
       </c>
-      <c r="E33" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" s="42" t="s">
+      <c r="E33" s="23">
+        <v>1</v>
+      </c>
+      <c r="F33" s="32" t="s">
         <v>4</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="9" customHeight="1">
@@ -1580,15 +1598,17 @@
       <c r="D35" s="23">
         <v>0.5</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="32" t="s">
-        <v>58</v>
+      <c r="E35" s="23">
+        <v>1</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>4</v>
       </c>
       <c r="G35" s="23"/>
     </row>
     <row r="36" spans="1:7" ht="8.5500000000000007" customHeight="1">
       <c r="A36" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>1</v>
@@ -1606,87 +1626,173 @@
       <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" ht="9" customHeight="1">
-      <c r="A37" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="38"/>
+      <c r="A37" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="35"/>
     </row>
     <row r="38" spans="1:7" ht="8.5500000000000007" customHeight="1">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
+      <c r="A38" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="23">
+        <v>0.5</v>
+      </c>
       <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
+      <c r="F38" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="8.6999999999999993" customHeight="1">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
+      <c r="A39" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="24">
+        <v>0.5</v>
+      </c>
       <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
+      <c r="F39" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G39" s="24" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="8.6999999999999993" customHeight="1">
-      <c r="A40" s="24"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
+      <c r="A40" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="24">
+        <v>1</v>
+      </c>
       <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
+      <c r="F40" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G40" s="24" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="8.6999999999999993" customHeight="1">
-      <c r="A41" s="24"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
+      <c r="A41" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="24">
+        <v>1.5</v>
+      </c>
       <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
+      <c r="F41" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="8.6999999999999993" customHeight="1">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
+      <c r="A42" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="24">
+        <v>2</v>
+      </c>
       <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
+      <c r="F42" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" s="24" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="8.6999999999999993" customHeight="1">
-      <c r="A43" s="24"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
+      <c r="A43" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="24">
+        <v>1</v>
+      </c>
       <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
+      <c r="F43" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" s="24" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="8.6999999999999993" customHeight="1">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
+      <c r="A44" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="24">
+        <v>1.5</v>
+      </c>
       <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-    </row>
-    <row r="45" spans="1:7" ht="8.6999999999999993" customHeight="1">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
+      <c r="F44" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G44" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="9" customHeight="1">
+      <c r="A45" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="35"/>
     </row>
     <row r="46" spans="1:7" ht="8.6999999999999993" customHeight="1">
       <c r="A46" s="24"/>
@@ -1725,7 +1831,8 @@
       <c r="G49" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A45:G45"/>
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="A37:G37"/>
     <mergeCell ref="A6:G6"/>

</xml_diff>

<commit_message>
status tracker update (week 6-7)
</commit_message>
<xml_diff>
--- a/docs/status tracker.xlsx
+++ b/docs/status tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1119DA8-4ADC-4123-988B-02F4CBD2E3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D539E56-6CE9-48CF-97AC-DB2330D72300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="83">
   <si>
     <r>
       <rPr>
@@ -283,6 +283,30 @@
   </si>
   <si>
     <t>Week 7 (February 26-March 3 )</t>
+  </si>
+  <si>
+    <t>Css Part of the pages</t>
+  </si>
+  <si>
+    <t>Attach backend with the frontend</t>
+  </si>
+  <si>
+    <t>Aditya,Aniket</t>
+  </si>
+  <si>
+    <t>Minor changes in the Page</t>
+  </si>
+  <si>
+    <t>Agrim,Shivam</t>
+  </si>
+  <si>
+    <t>Do CSS part of the pages made</t>
+  </si>
+  <si>
+    <t>Connect the backend from local to mongodb atlas</t>
+  </si>
+  <si>
+    <t>Make some changes in purchase and status tracker page</t>
   </si>
 </sst>
 </file>
@@ -943,10 +967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999"/>
@@ -1649,9 +1673,11 @@
       <c r="D38" s="23">
         <v>0.5</v>
       </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23" t="s">
-        <v>55</v>
+      <c r="E38" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G38" s="23" t="s">
         <v>67</v>
@@ -1670,9 +1696,11 @@
       <c r="D39" s="24">
         <v>0.5</v>
       </c>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24" t="s">
-        <v>55</v>
+      <c r="E39" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G39" s="24" t="s">
         <v>38</v>
@@ -1691,9 +1719,11 @@
       <c r="D40" s="24">
         <v>1</v>
       </c>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24" t="s">
-        <v>55</v>
+      <c r="E40" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G40" s="24" t="s">
         <v>68</v>
@@ -1712,9 +1742,11 @@
       <c r="D41" s="24">
         <v>1.5</v>
       </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24" t="s">
-        <v>55</v>
+      <c r="E41" s="24">
+        <v>2</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G41" s="24" t="s">
         <v>69</v>
@@ -1733,9 +1765,11 @@
       <c r="D42" s="24">
         <v>2</v>
       </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24" t="s">
-        <v>55</v>
+      <c r="E42" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G42" s="24" t="s">
         <v>70</v>
@@ -1754,9 +1788,11 @@
       <c r="D43" s="24">
         <v>1</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
-        <v>55</v>
+      <c r="E43" s="24">
+        <v>2.5</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G43" s="24" t="s">
         <v>71</v>
@@ -1775,9 +1811,11 @@
       <c r="D44" s="24">
         <v>1.5</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
-        <v>55</v>
+      <c r="E44" s="24">
+        <v>1</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G44" s="24" t="s">
         <v>72</v>
@@ -1794,41 +1832,129 @@
       <c r="F45" s="34"/>
       <c r="G45" s="35"/>
     </row>
-    <row r="46" spans="1:7" ht="8.6999999999999993" customHeight="1">
-      <c r="A46" s="24"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
+    <row r="46" spans="1:7" ht="8.5500000000000007" customHeight="1">
+      <c r="A46" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="8.6999999999999993" customHeight="1">
-      <c r="A47" s="24"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
+      <c r="A47" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="24">
+        <v>0.5</v>
+      </c>
       <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
+      <c r="F47" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" s="24" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="8.6999999999999993" customHeight="1">
-      <c r="A48" s="24"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
+      <c r="A48" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="24">
+        <v>1</v>
+      </c>
       <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
+      <c r="F48" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G48" s="24" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="8.5500000000000007" customHeight="1">
-      <c r="A49" s="24"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
+      <c r="A49" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D49" s="24">
+        <v>2</v>
+      </c>
       <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
+      <c r="F49" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="9">
+        <v>2</v>
+      </c>
+      <c r="F50" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="9">
+        <v>1</v>
+      </c>
+      <c r="F51" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
status tracker week 8
</commit_message>
<xml_diff>
--- a/docs/status tracker.xlsx
+++ b/docs/status tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D539E56-6CE9-48CF-97AC-DB2330D72300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE4CFD9-59E6-4144-A000-4A9CB2AEDA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="95">
   <si>
     <r>
       <rPr>
@@ -307,6 +307,42 @@
   </si>
   <si>
     <t>Make some changes in purchase and status tracker page</t>
+  </si>
+  <si>
+    <t>Update status tracker page</t>
+  </si>
+  <si>
+    <t>Add downloadable files in backend</t>
+  </si>
+  <si>
+    <t>Css and animation</t>
+  </si>
+  <si>
+    <t>Shivam,Atidipt</t>
+  </si>
+  <si>
+    <t>Make changes in the status tracker page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upload downloadable files in backend </t>
+  </si>
+  <si>
+    <t>Add css and animation in the website</t>
+  </si>
+  <si>
+    <t>Live testing</t>
+  </si>
+  <si>
+    <t>Check each functionality with the client</t>
+  </si>
+  <si>
+    <t>Give updates about the work, and do live testing</t>
+  </si>
+  <si>
+    <t>Week 8  (March 4-March 10 )</t>
+  </si>
+  <si>
+    <t>Week 9  (March 11-March 17  )</t>
   </si>
 </sst>
 </file>
@@ -358,7 +394,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +429,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -524,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -640,6 +682,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -967,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999"/>
@@ -1845,9 +1890,11 @@
       <c r="D46" s="23">
         <v>0.5</v>
       </c>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23" t="s">
-        <v>55</v>
+      <c r="E46" s="23">
+        <v>3</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G46" s="23" t="s">
         <v>67</v>
@@ -1861,14 +1908,16 @@
         <v>36</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D47" s="24">
         <v>0.5</v>
       </c>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24" t="s">
-        <v>55</v>
+      <c r="E47" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G47" s="24" t="s">
         <v>38</v>
@@ -1887,9 +1936,11 @@
       <c r="D48" s="24">
         <v>1</v>
       </c>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24" t="s">
-        <v>55</v>
+      <c r="E48" s="24">
+        <v>1</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G48" s="24" t="s">
         <v>68</v>
@@ -1908,9 +1959,11 @@
       <c r="D49" s="24">
         <v>2</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24" t="s">
-        <v>55</v>
+      <c r="E49" s="24">
+        <v>2.5</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>3</v>
       </c>
       <c r="G49" s="24" t="s">
         <v>80</v>
@@ -1929,8 +1982,11 @@
       <c r="D50" s="9">
         <v>2</v>
       </c>
-      <c r="F50" s="24" t="s">
-        <v>55</v>
+      <c r="E50" s="9">
+        <v>4</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>81</v>
@@ -1949,15 +2005,185 @@
       <c r="D51" s="9">
         <v>1</v>
       </c>
-      <c r="F51" s="24" t="s">
-        <v>55</v>
+      <c r="E51" s="9">
+        <v>2</v>
+      </c>
+      <c r="F51" s="31" t="s">
+        <v>3</v>
       </c>
       <c r="G51" s="9" t="s">
         <v>82</v>
       </c>
     </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="35"/>
+    </row>
+    <row r="53" spans="1:7" ht="8.5500000000000007" customHeight="1">
+      <c r="A53" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E53" s="23"/>
+      <c r="F53" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="G53" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="8.6999999999999993" customHeight="1">
+      <c r="A54" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="E54" s="24"/>
+      <c r="F54" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="G54" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="8.6999999999999993" customHeight="1">
+      <c r="A55" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="24">
+        <v>1</v>
+      </c>
+      <c r="E55" s="24"/>
+      <c r="F55" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="G55" s="24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" s="9">
+        <v>2</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D58" s="9">
+        <v>2</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="9">
+        <v>1</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="35"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A60:G60"/>
     <mergeCell ref="A45:G45"/>
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="A37:G37"/>

</xml_diff>

<commit_message>
status tracker week-8, 9
gargy garg
</commit_message>
<xml_diff>
--- a/docs/status tracker.xlsx
+++ b/docs/status tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE4CFD9-59E6-4144-A000-4A9CB2AEDA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0788C67B-BC41-4598-9E09-FB4E967A7BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="105">
   <si>
     <r>
       <rPr>
@@ -343,6 +343,36 @@
   </si>
   <si>
     <t>Week 9  (March 11-March 17  )</t>
+  </si>
+  <si>
+    <t>Local host to local server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add authentication routing </t>
+  </si>
+  <si>
+    <t>Complete status tracker page</t>
+  </si>
+  <si>
+    <t>Adding downlodable files on webpage</t>
+  </si>
+  <si>
+    <t>Aniket,Atidipt</t>
+  </si>
+  <si>
+    <t>The local host could be seen from any device</t>
+  </si>
+  <si>
+    <t>Once the user is logged in then only redirect to other pages</t>
+  </si>
+  <si>
+    <t>Add various columns and actions in status tracker page</t>
+  </si>
+  <si>
+    <t>Add downloadable links in status tracker page</t>
+  </si>
+  <si>
+    <t>Week 10  (March 18-March 24  )</t>
   </si>
 </sst>
 </file>
@@ -666,6 +696,9 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -682,9 +715,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1012,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999"/>
@@ -1102,26 +1132,26 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" spans="1:7" ht="9" customHeight="1">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7" ht="9" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -1225,15 +1255,15 @@
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="9" customHeight="1">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" spans="1:7" ht="9" customHeight="1">
       <c r="A14" s="4" t="s">
@@ -1383,15 +1413,15 @@
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="9" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="35"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="1:7" ht="9" customHeight="1">
       <c r="A22" s="4" t="s">
@@ -1509,15 +1539,15 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="9" customHeight="1">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="35"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" spans="1:7" ht="8.5500000000000007" customHeight="1">
       <c r="A28" s="23" t="s">
@@ -1598,15 +1628,15 @@
       <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:7" ht="9" customHeight="1">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" spans="1:7" ht="9" customHeight="1">
       <c r="A33" s="4" t="s">
@@ -1695,15 +1725,15 @@
       <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" ht="9" customHeight="1">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="35"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" spans="1:7" ht="8.5500000000000007" customHeight="1">
       <c r="A38" s="23" t="s">
@@ -1867,15 +1897,15 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="9" customHeight="1">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="35"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="36"/>
     </row>
     <row r="46" spans="1:7" ht="8.5500000000000007" customHeight="1">
       <c r="A46" s="23" t="s">
@@ -2016,15 +2046,15 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="33" t="s">
+      <c r="A52" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="35"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="36"/>
     </row>
     <row r="53" spans="1:7" ht="8.5500000000000007" customHeight="1">
       <c r="A53" s="23" t="s">
@@ -2039,9 +2069,11 @@
       <c r="D53" s="23">
         <v>0.5</v>
       </c>
-      <c r="E53" s="23"/>
-      <c r="F53" s="39" t="s">
-        <v>55</v>
+      <c r="E53" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G53" s="23" t="s">
         <v>92</v>
@@ -2060,9 +2092,11 @@
       <c r="D54" s="24">
         <v>0.5</v>
       </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="39" t="s">
-        <v>55</v>
+      <c r="E54" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G54" s="24" t="s">
         <v>38</v>
@@ -2081,9 +2115,11 @@
       <c r="D55" s="24">
         <v>1</v>
       </c>
-      <c r="E55" s="24"/>
-      <c r="F55" s="39" t="s">
-        <v>55</v>
+      <c r="E55" s="24">
+        <v>1</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G55" s="24" t="s">
         <v>68</v>
@@ -2102,8 +2138,8 @@
       <c r="D56" s="9">
         <v>2</v>
       </c>
-      <c r="F56" s="9" t="s">
-        <v>55</v>
+      <c r="F56" s="31" t="s">
+        <v>3</v>
       </c>
       <c r="G56" s="9" t="s">
         <v>87</v>
@@ -2122,8 +2158,8 @@
       <c r="D57" s="9">
         <v>2.5</v>
       </c>
-      <c r="F57" s="9" t="s">
-        <v>55</v>
+      <c r="F57" s="31" t="s">
+        <v>3</v>
       </c>
       <c r="G57" s="9" t="s">
         <v>88</v>
@@ -2142,8 +2178,11 @@
       <c r="D58" s="9">
         <v>2</v>
       </c>
-      <c r="F58" s="9" t="s">
-        <v>55</v>
+      <c r="E58" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G58" s="9" t="s">
         <v>89</v>
@@ -2162,36 +2201,194 @@
       <c r="D59" s="9">
         <v>1</v>
       </c>
-      <c r="F59" s="9" t="s">
-        <v>55</v>
+      <c r="E59" s="9">
+        <v>1</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G59" s="9" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="33" t="s">
+      <c r="A60" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="35"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="36"/>
+    </row>
+    <row r="61" spans="1:7" ht="8.5500000000000007" customHeight="1">
+      <c r="A61" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E61" s="23"/>
+      <c r="F61" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="8.6999999999999993" customHeight="1">
+      <c r="A62" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="E62" s="24"/>
+      <c r="F62" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G62" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="8.6999999999999993" customHeight="1">
+      <c r="A63" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="24">
+        <v>1</v>
+      </c>
+      <c r="E63" s="24"/>
+      <c r="F63" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G63" s="24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="F64" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D65" s="9">
+        <v>2</v>
+      </c>
+      <c r="F65" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B66" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" s="9">
+        <v>2</v>
+      </c>
+      <c r="F66" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B67" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="F67" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A68:G68"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A27:G27"/>
     <mergeCell ref="A52:G52"/>
     <mergeCell ref="A60:G60"/>
     <mergeCell ref="A45:G45"/>
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A27:G27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
status tracker week 9-10
</commit_message>
<xml_diff>
--- a/docs/status tracker.xlsx
+++ b/docs/status tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0788C67B-BC41-4598-9E09-FB4E967A7BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04600D26-8AA6-4D8E-AFC3-143F41E8D22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="116">
   <si>
     <r>
       <rPr>
@@ -373,6 +373,39 @@
   </si>
   <si>
     <t>Week 10  (March 18-March 24  )</t>
+  </si>
+  <si>
+    <t>Cancelled by client</t>
+  </si>
+  <si>
+    <t>R1 Presentation</t>
+  </si>
+  <si>
+    <t>Updating all the live documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final testing before R1 </t>
+  </si>
+  <si>
+    <t>Preparation for R2</t>
+  </si>
+  <si>
+    <t>Aditya,Aniket,Agrim</t>
+  </si>
+  <si>
+    <t>Creating a presentation for R1</t>
+  </si>
+  <si>
+    <t>Updating All the live documents</t>
+  </si>
+  <si>
+    <t>Do a testing of the website before R1</t>
+  </si>
+  <si>
+    <t>Plan what all needs to be done in R2</t>
+  </si>
+  <si>
+    <t>Week 11  (March 25-March 31  )</t>
   </si>
 </sst>
 </file>
@@ -1042,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="149" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999"/>
@@ -1992,8 +2025,8 @@
       <c r="E49" s="24">
         <v>2.5</v>
       </c>
-      <c r="F49" s="31" t="s">
-        <v>3</v>
+      <c r="F49" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G49" s="24" t="s">
         <v>80</v>
@@ -2038,8 +2071,8 @@
       <c r="E51" s="9">
         <v>2</v>
       </c>
-      <c r="F51" s="31" t="s">
-        <v>3</v>
+      <c r="F51" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G51" s="9" t="s">
         <v>82</v>
@@ -2138,8 +2171,8 @@
       <c r="D56" s="9">
         <v>2</v>
       </c>
-      <c r="F56" s="31" t="s">
-        <v>3</v>
+      <c r="F56" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G56" s="9" t="s">
         <v>87</v>
@@ -2236,11 +2269,11 @@
         <v>0.5</v>
       </c>
       <c r="E61" s="23"/>
-      <c r="F61" s="33" t="s">
-        <v>55</v>
+      <c r="F61" s="29" t="s">
+        <v>2</v>
       </c>
       <c r="G61" s="23" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="8.6999999999999993" customHeight="1">
@@ -2256,9 +2289,11 @@
       <c r="D62" s="24">
         <v>0.5</v>
       </c>
-      <c r="E62" s="24"/>
-      <c r="F62" s="33" t="s">
-        <v>55</v>
+      <c r="E62" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="F62" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G62" s="24" t="s">
         <v>38</v>
@@ -2277,9 +2312,11 @@
       <c r="D63" s="24">
         <v>1</v>
       </c>
-      <c r="E63" s="24"/>
-      <c r="F63" s="33" t="s">
-        <v>55</v>
+      <c r="E63" s="24">
+        <v>1</v>
+      </c>
+      <c r="F63" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G63" s="24" t="s">
         <v>68</v>
@@ -2298,8 +2335,8 @@
       <c r="D64" s="9">
         <v>1.5</v>
       </c>
-      <c r="F64" s="33" t="s">
-        <v>55</v>
+      <c r="F64" s="31" t="s">
+        <v>3</v>
       </c>
       <c r="G64" s="9" t="s">
         <v>100</v>
@@ -2318,8 +2355,11 @@
       <c r="D65" s="9">
         <v>2</v>
       </c>
-      <c r="F65" s="33" t="s">
-        <v>55</v>
+      <c r="E65" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="F65" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G65" s="9" t="s">
         <v>101</v>
@@ -2338,8 +2378,11 @@
       <c r="D66" s="9">
         <v>2</v>
       </c>
-      <c r="F66" s="33" t="s">
-        <v>55</v>
+      <c r="E66" s="9">
+        <v>3</v>
+      </c>
+      <c r="F66" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G66" s="9" t="s">
         <v>102</v>
@@ -2358,8 +2401,8 @@
       <c r="D67" s="9">
         <v>2.5</v>
       </c>
-      <c r="F67" s="33" t="s">
-        <v>55</v>
+      <c r="F67" s="31" t="s">
+        <v>3</v>
       </c>
       <c r="G67" s="9" t="s">
         <v>103</v>
@@ -2376,8 +2419,163 @@
       <c r="F68" s="35"/>
       <c r="G68" s="36"/>
     </row>
+    <row r="69" spans="1:7" ht="8.5500000000000007" customHeight="1">
+      <c r="A69" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E69" s="23"/>
+      <c r="F69" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G69" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="8.6999999999999993" customHeight="1">
+      <c r="A70" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D70" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="E70" s="24"/>
+      <c r="F70" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="8.6999999999999993" customHeight="1">
+      <c r="A71" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="24">
+        <v>1</v>
+      </c>
+      <c r="E71" s="24"/>
+      <c r="F71" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G71" s="24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72" s="9">
+        <v>2</v>
+      </c>
+      <c r="F72" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D73" s="9">
+        <v>2</v>
+      </c>
+      <c r="F73" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="F74" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="9">
+        <v>3</v>
+      </c>
+      <c r="F75" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B76" s="35"/>
+      <c r="C76" s="35"/>
+      <c r="D76" s="35"/>
+      <c r="E76" s="35"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="36"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A76:G76"/>
     <mergeCell ref="A68:G68"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A7:G7"/>

</xml_diff>

<commit_message>
changed status tracker 24-03-2024
Gargy Garg
</commit_message>
<xml_diff>
--- a/docs/status tracker.xlsx
+++ b/docs/status tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04600D26-8AA6-4D8E-AFC3-143F41E8D22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD57EBE-319F-4246-AAE1-50A43FC04DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="124">
   <si>
     <r>
       <rPr>
@@ -406,6 +406,30 @@
   </si>
   <si>
     <t>Week 11  (March 25-March 31  )</t>
+  </si>
+  <si>
+    <t>Client Office visit</t>
+  </si>
+  <si>
+    <t>Status Tracker Page update</t>
+  </si>
+  <si>
+    <t>Start working on R2</t>
+  </si>
+  <si>
+    <t>Visit the client office and get insights of project</t>
+  </si>
+  <si>
+    <t>Add few options in status tracker page</t>
+  </si>
+  <si>
+    <t>Check all the purchase functionality</t>
+  </si>
+  <si>
+    <t>Plan and divide each work for R2</t>
+  </si>
+  <si>
+    <t>Week 12  (April 01-April 07  )</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="149" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="149" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999"/>
@@ -2432,9 +2456,11 @@
       <c r="D69" s="23">
         <v>0.5</v>
       </c>
-      <c r="E69" s="23"/>
-      <c r="F69" s="33" t="s">
-        <v>55</v>
+      <c r="E69" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="F69" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G69" s="23" t="s">
         <v>105</v>
@@ -2453,9 +2479,11 @@
       <c r="D70" s="24">
         <v>0.5</v>
       </c>
-      <c r="E70" s="24"/>
-      <c r="F70" s="33" t="s">
-        <v>55</v>
+      <c r="E70" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="F70" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G70" s="24" t="s">
         <v>38</v>
@@ -2474,9 +2502,11 @@
       <c r="D71" s="24">
         <v>1</v>
       </c>
-      <c r="E71" s="24"/>
-      <c r="F71" s="33" t="s">
-        <v>55</v>
+      <c r="E71" s="24">
+        <v>2</v>
+      </c>
+      <c r="F71" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G71" s="24" t="s">
         <v>68</v>
@@ -2495,8 +2525,11 @@
       <c r="D72" s="9">
         <v>2</v>
       </c>
-      <c r="F72" s="33" t="s">
-        <v>55</v>
+      <c r="E72" s="9">
+        <v>3</v>
+      </c>
+      <c r="F72" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G72" s="9" t="s">
         <v>111</v>
@@ -2515,8 +2548,11 @@
       <c r="D73" s="9">
         <v>2</v>
       </c>
-      <c r="F73" s="33" t="s">
-        <v>55</v>
+      <c r="E73" s="9">
+        <v>2</v>
+      </c>
+      <c r="F73" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G73" s="9" t="s">
         <v>112</v>
@@ -2535,8 +2571,11 @@
       <c r="D74" s="9">
         <v>1.5</v>
       </c>
-      <c r="F74" s="33" t="s">
-        <v>55</v>
+      <c r="E74" s="9">
+        <v>1</v>
+      </c>
+      <c r="F74" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="G74" s="9" t="s">
         <v>113</v>
@@ -2555,8 +2594,8 @@
       <c r="D75" s="9">
         <v>3</v>
       </c>
-      <c r="F75" s="33" t="s">
-        <v>55</v>
+      <c r="F75" s="31" t="s">
+        <v>3</v>
       </c>
       <c r="G75" s="9" t="s">
         <v>114</v>
@@ -2573,8 +2612,163 @@
       <c r="F76" s="35"/>
       <c r="G76" s="36"/>
     </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E77" s="23"/>
+      <c r="F77" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G77" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D78" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="E78" s="24"/>
+      <c r="F78" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G78" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="20.399999999999999">
+      <c r="A79" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="24">
+        <v>1</v>
+      </c>
+      <c r="E79" s="24"/>
+      <c r="F79" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G79" s="24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B80" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="9">
+        <v>4</v>
+      </c>
+      <c r="F80" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" s="9">
+        <v>2</v>
+      </c>
+      <c r="F81" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="9">
+        <v>1</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="9">
+        <v>2</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B84" s="35"/>
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
+      <c r="E84" s="35"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="36"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A84:G84"/>
     <mergeCell ref="A76:G76"/>
     <mergeCell ref="A68:G68"/>
     <mergeCell ref="A6:G6"/>

</xml_diff>